<commit_message>
Fix intégration MDD + Module OE + Download images et documents PDF
</commit_message>
<xml_diff>
--- a/INPUT/CEDILOG.xlsx
+++ b/INPUT/CEDILOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects2\MDD\INPUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636AB1E1-4D2F-465B-A579-9513DA08B1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF47C84-2D89-48F6-8B3E-10D4EF13585E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="4104" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CROSS" sheetId="1" r:id="rId1"/>
@@ -5542,126 +5542,126 @@
   <dimension ref="A1:DJ439"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="49.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="33.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.7265625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="33.7265625" style="1" customWidth="1"/>
     <col min="12" max="13" width="36" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="115" max="16384" width="14.7109375" style="1"/>
+    <col min="14" max="14" width="28.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="48.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="115" max="16384" width="14.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:114" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:114" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>836</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>842</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>845</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>850</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>646</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>648</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>649</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>650</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>651</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>652</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>760</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>761</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>846</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>851</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:114" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:114" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>859</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>860</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>861</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>863</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>865</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>866</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>653</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>655</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>879</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>882</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>656</v>
       </c>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>658</v>
       </c>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>758</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>759</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>824</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>825</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>757</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>756</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>862</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>864</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>785</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>786</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>787</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>788</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>789</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>790</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>867</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>868</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>791</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>792</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>659</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>661</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>869</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>870</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>871</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>872</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>873</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>874</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>793</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>794</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>662</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>664</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>875</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>876</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>755</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>753</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>877</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>835</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>795</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>796</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>797</v>
       </c>
@@ -8162,7 +8162,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>798</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>799</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>801</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>665</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>666</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>667</v>
       </c>
@@ -8372,7 +8372,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>669</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>670</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>672</v>
       </c>
@@ -8477,7 +8477,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>673</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>675</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>676</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>677</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
         <v>678</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>679</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>680</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>682</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
         <v>683</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>684</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
         <v>685</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
         <v>687</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>688</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
         <v>690</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>838</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>40175049</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>843</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>40175050</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>847</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>40175072</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>852</v>
       </c>
@@ -8951,7 +8951,7 @@
         <v>40175073</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
         <v>855</v>
       </c>
@@ -8974,7 +8974,7 @@
         <v>5001852882</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>856</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>5001852883</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>857</v>
       </c>
@@ -9014,7 +9014,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
         <v>858</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>802</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>40195037</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>804</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>40195038</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>848</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>40195011</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
         <v>853</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>40195012</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A102" s="7" t="s">
         <v>832</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>40195021</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A103" s="7" t="s">
         <v>781</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>40195022</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104" s="7" t="s">
         <v>828</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>40195045</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
         <v>829</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>40195046</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
         <v>780</v>
       </c>
@@ -9238,7 +9238,7 @@
         <v>640195068</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107" s="7" t="s">
         <v>691</v>
       </c>
@@ -9261,7 +9261,7 @@
         <v>640195069</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108" s="7" t="s">
         <v>840</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>40225003</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
         <v>844</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>40225004</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110" s="7" t="s">
         <v>849</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>40225015</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111" s="7" t="s">
         <v>854</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>40225016</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
         <v>693</v>
       </c>
@@ -9376,7 +9376,7 @@
         <v>640225030</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113" s="7" t="s">
         <v>695</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>640225031</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
         <v>696</v>
       </c>
@@ -9422,7 +9422,7 @@
         <v>640225025</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
         <v>697</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>640225023</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A116" s="7" t="s">
         <v>698</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>40465019</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A117" s="7" t="s">
         <v>700</v>
       </c>
@@ -9491,7 +9491,7 @@
         <v>40465019</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A118" s="7" t="s">
         <v>878</v>
       </c>
@@ -9521,7 +9521,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A119" s="7" t="s">
         <v>881</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A120" s="7" t="s">
         <v>883</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
         <v>884</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A122" s="7" t="s">
         <v>885</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A123" s="7" t="s">
         <v>886</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A124" s="7" t="s">
         <v>701</v>
       </c>
@@ -9690,7 +9690,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A125" s="7" t="s">
         <v>887</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A126" s="7" t="s">
         <v>888</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A127" s="7" t="s">
         <v>889</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A128" s="7" t="s">
         <v>890</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A129" s="7" t="s">
         <v>891</v>
       </c>
@@ -9817,7 +9817,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A130" s="7" t="s">
         <v>892</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A131" s="7" t="s">
         <v>893</v>
       </c>
@@ -9875,7 +9875,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A132" s="7" t="s">
         <v>894</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A133" s="7" t="s">
         <v>895</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A134" s="7" t="s">
         <v>896</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A135" s="7" t="s">
         <v>897</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
         <v>898</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A137" s="7" t="s">
         <v>899</v>
       </c>
@@ -10025,7 +10025,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A138" s="7" t="s">
         <v>830</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A139" s="7" t="s">
         <v>900</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A140" s="7" t="s">
         <v>901</v>
       </c>
@@ -10094,7 +10094,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
         <v>903</v>
       </c>
@@ -10117,7 +10117,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A142" s="7" t="s">
         <v>911</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A143" s="7" t="s">
         <v>912</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A144" s="7" t="s">
         <v>915</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A145" s="7" t="s">
         <v>916</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A146" s="7" t="s">
         <v>953</v>
       </c>
@@ -10239,7 +10239,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" s="7" t="s">
         <v>954</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A148" s="7" t="s">
         <v>955</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A149" s="7" t="s">
         <v>956</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A150" s="7" t="s">
         <v>957</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A151" s="7" t="s">
         <v>958</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A152" s="7" t="s">
         <v>959</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A153" s="7" t="s">
         <v>960</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A154" s="7" t="s">
         <v>961</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A155" s="7" t="s">
         <v>962</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A156" s="7" t="s">
         <v>703</v>
       </c>
@@ -10520,7 +10520,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A157" s="7" t="s">
         <v>705</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A158" s="7" t="s">
         <v>963</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A159" s="7" t="s">
         <v>964</v>
       </c>
@@ -10607,7 +10607,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A160" s="7" t="s">
         <v>969</v>
       </c>
@@ -10630,7 +10630,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A161" s="7" t="s">
         <v>970</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A162" s="7" t="s">
         <v>971</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A163" s="7" t="s">
         <v>831</v>
       </c>
@@ -10713,7 +10713,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A164" s="7" t="s">
         <v>978</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A165" s="7" t="s">
         <v>979</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A166" s="7" t="s">
         <v>904</v>
       </c>
@@ -10788,7 +10788,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A167" s="7" t="s">
         <v>906</v>
       </c>
@@ -10817,7 +10817,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A168" s="7" t="s">
         <v>907</v>
       </c>
@@ -10846,7 +10846,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A169" s="7" t="s">
         <v>908</v>
       </c>
@@ -10875,7 +10875,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A170" s="7" t="s">
         <v>909</v>
       </c>
@@ -10904,7 +10904,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A171" s="7" t="s">
         <v>910</v>
       </c>
@@ -10933,7 +10933,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A172" s="7" t="s">
         <v>913</v>
       </c>
@@ -10962,7 +10962,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A173" s="7" t="s">
         <v>914</v>
       </c>
@@ -10991,7 +10991,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A174" s="7" t="s">
         <v>931</v>
       </c>
@@ -11021,7 +11021,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A175" s="7" t="s">
         <v>932</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A176" s="7" t="s">
         <v>967</v>
       </c>
@@ -11079,7 +11079,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A177" s="7" t="s">
         <v>968</v>
       </c>
@@ -11108,7 +11108,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A178" s="7" t="s">
         <v>772</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A179" s="7" t="s">
         <v>770</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A180" s="7" t="s">
         <v>920</v>
       </c>
@@ -11195,7 +11195,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A181" s="7" t="s">
         <v>921</v>
       </c>
@@ -11224,7 +11224,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A182" s="7" t="s">
         <v>925</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A183" s="7" t="s">
         <v>927</v>
       </c>
@@ -11282,7 +11282,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A184" s="7" t="s">
         <v>949</v>
       </c>
@@ -11311,7 +11311,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A185" s="7" t="s">
         <v>950</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A186" s="7" t="s">
         <v>951</v>
       </c>
@@ -11370,7 +11370,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A187" s="7" t="s">
         <v>952</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A188" s="7" t="s">
         <v>972</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A189" s="7" t="s">
         <v>973</v>
       </c>
@@ -11460,7 +11460,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A190" s="7" t="s">
         <v>805</v>
       </c>
@@ -11489,7 +11489,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A191" s="7" t="s">
         <v>806</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A192" s="7" t="s">
         <v>922</v>
       </c>
@@ -11547,7 +11547,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A193" s="7" t="s">
         <v>924</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A194" s="7" t="s">
         <v>928</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A195" s="7" t="s">
         <v>930</v>
       </c>
@@ -11634,7 +11634,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A196" s="7" t="s">
         <v>939</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A197" s="7" t="s">
         <v>940</v>
       </c>
@@ -11692,7 +11692,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A198" s="7" t="s">
         <v>807</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A199" s="7" t="s">
         <v>808</v>
       </c>
@@ -11750,7 +11750,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A200" s="7" t="s">
         <v>776</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A201" s="7" t="s">
         <v>778</v>
       </c>
@@ -11808,7 +11808,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A202" s="7" t="s">
         <v>982</v>
       </c>
@@ -11837,7 +11837,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A203" s="7" t="s">
         <v>983</v>
       </c>
@@ -11866,7 +11866,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A204" s="7" t="s">
         <v>833</v>
       </c>
@@ -11895,7 +11895,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A205" s="7" t="s">
         <v>984</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A206" s="7" t="s">
         <v>809</v>
       </c>
@@ -11959,7 +11959,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A207" s="7" t="s">
         <v>811</v>
       </c>
@@ -11994,7 +11994,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A208" s="7" t="s">
         <v>917</v>
       </c>
@@ -12023,7 +12023,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A209" s="7" t="s">
         <v>779</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A210" s="7" t="s">
         <v>933</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A211" s="7" t="s">
         <v>934</v>
       </c>
@@ -12110,7 +12110,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A212" s="7" t="s">
         <v>935</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A213" s="7" t="s">
         <v>936</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A214" s="7" t="s">
         <v>937</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A215" s="7" t="s">
         <v>938</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A216" s="7" t="s">
         <v>945</v>
       </c>
@@ -12257,7 +12257,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A217" s="7" t="s">
         <v>946</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A218" s="7" t="s">
         <v>947</v>
       </c>
@@ -12315,7 +12315,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A219" s="7" t="s">
         <v>948</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A220" s="7" t="s">
         <v>812</v>
       </c>
@@ -12373,7 +12373,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A221" s="7" t="s">
         <v>813</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A222" s="7" t="s">
         <v>965</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A223" s="7" t="s">
         <v>966</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A224" s="7" t="s">
         <v>974</v>
       </c>
@@ -12489,7 +12489,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A225" s="7" t="s">
         <v>975</v>
       </c>
@@ -12518,7 +12518,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A226" s="7" t="s">
         <v>769</v>
       </c>
@@ -12547,7 +12547,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A227" s="7" t="s">
         <v>767</v>
       </c>
@@ -12576,7 +12576,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A228" s="7" t="s">
         <v>990</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A229" s="7" t="s">
         <v>991</v>
       </c>
@@ -12634,7 +12634,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A230" s="7" t="s">
         <v>1004</v>
       </c>
@@ -12664,7 +12664,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A231" s="7" t="s">
         <v>1005</v>
       </c>
@@ -12694,7 +12694,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A232" s="7" t="s">
         <v>826</v>
       </c>
@@ -12723,7 +12723,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A233" s="7" t="s">
         <v>827</v>
       </c>
@@ -12752,7 +12752,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A234" s="7" t="s">
         <v>918</v>
       </c>
@@ -12781,7 +12781,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A235" s="7" t="s">
         <v>919</v>
       </c>
@@ -12810,7 +12810,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A236" s="7" t="s">
         <v>766</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A237" s="7" t="s">
         <v>765</v>
       </c>
@@ -12868,7 +12868,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A238" s="7" t="s">
         <v>941</v>
       </c>
@@ -12897,7 +12897,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A239" s="7" t="s">
         <v>942</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A240" s="7" t="s">
         <v>943</v>
       </c>
@@ -12955,7 +12955,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A241" s="7" t="s">
         <v>944</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A242" s="7" t="s">
         <v>976</v>
       </c>
@@ -13013,7 +13013,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A243" s="7" t="s">
         <v>977</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A244" s="7" t="s">
         <v>980</v>
       </c>
@@ -13071,7 +13071,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A245" s="7" t="s">
         <v>981</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A246" s="7" t="s">
         <v>814</v>
       </c>
@@ -13129,7 +13129,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A247" s="7" t="s">
         <v>815</v>
       </c>
@@ -13158,7 +13158,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A248" s="7" t="s">
         <v>816</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A249" s="7" t="s">
         <v>706</v>
       </c>
@@ -13216,7 +13216,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A250" s="7" t="s">
         <v>817</v>
       </c>
@@ -13245,7 +13245,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A251" s="7" t="s">
         <v>708</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A252" s="7" t="s">
         <v>985</v>
       </c>
@@ -13303,7 +13303,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A253" s="7" t="s">
         <v>986</v>
       </c>
@@ -13332,7 +13332,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A254" s="7" t="s">
         <v>987</v>
       </c>
@@ -13361,7 +13361,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A255" s="7" t="s">
         <v>709</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A256" s="7" t="s">
         <v>988</v>
       </c>
@@ -13419,7 +13419,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A257" s="7" t="s">
         <v>710</v>
       </c>
@@ -13448,7 +13448,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A258" s="7" t="s">
         <v>764</v>
       </c>
@@ -13477,7 +13477,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A259" s="7" t="s">
         <v>762</v>
       </c>
@@ -13506,7 +13506,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A260" s="7" t="s">
         <v>818</v>
       </c>
@@ -13535,7 +13535,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A261" s="7" t="s">
         <v>819</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A262" s="7" t="s">
         <v>992</v>
       </c>
@@ -13593,7 +13593,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A263" s="7" t="s">
         <v>993</v>
       </c>
@@ -13622,7 +13622,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A264" s="7" t="s">
         <v>994</v>
       </c>
@@ -13651,7 +13651,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A265" s="7" t="s">
         <v>995</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A266" s="7" t="s">
         <v>996</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A267" s="7" t="s">
         <v>997</v>
       </c>
@@ -13738,7 +13738,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A268" s="7" t="s">
         <v>784</v>
       </c>
@@ -13767,7 +13767,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A269" s="7" t="s">
         <v>711</v>
       </c>
@@ -13796,7 +13796,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A270" s="7" t="s">
         <v>783</v>
       </c>
@@ -13825,7 +13825,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A271" s="7" t="s">
         <v>712</v>
       </c>
@@ -13854,7 +13854,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A272" s="7" t="s">
         <v>1000</v>
       </c>
@@ -13883,7 +13883,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A273" s="7" t="s">
         <v>1001</v>
       </c>
@@ -13912,7 +13912,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A274" s="7" t="s">
         <v>1002</v>
       </c>
@@ -13941,7 +13941,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A275" s="7" t="s">
         <v>1003</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A276" s="7" t="s">
         <v>775</v>
       </c>
@@ -13999,7 +13999,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A277" s="7" t="s">
         <v>713</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A278" s="7" t="s">
         <v>989</v>
       </c>
@@ -14057,7 +14057,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A279" s="7" t="s">
         <v>715</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A280" s="7" t="s">
         <v>998</v>
       </c>
@@ -14115,7 +14115,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A281" s="7" t="s">
         <v>999</v>
       </c>
@@ -14144,7 +14144,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A282" s="7" t="s">
         <v>716</v>
       </c>
@@ -14167,7 +14167,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A283" s="7" t="s">
         <v>718</v>
       </c>
@@ -14190,7 +14190,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A284" s="7" t="s">
         <v>719</v>
       </c>
@@ -14219,7 +14219,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A285" s="7" t="s">
         <v>720</v>
       </c>
@@ -14248,7 +14248,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A286" s="7" t="s">
         <v>721</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A287" s="7" t="s">
         <v>722</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A288" s="7" t="s">
         <v>723</v>
       </c>
@@ -14323,7 +14323,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A289" s="7" t="s">
         <v>724</v>
       </c>
@@ -14352,7 +14352,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A290" s="7" t="s">
         <v>820</v>
       </c>
@@ -14381,7 +14381,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A291" s="7" t="s">
         <v>821</v>
       </c>
@@ -14410,7 +14410,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A292" s="7" t="s">
         <v>822</v>
       </c>
@@ -14439,7 +14439,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A293" s="7" t="s">
         <v>725</v>
       </c>
@@ -14468,7 +14468,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A294" s="7" t="s">
         <v>823</v>
       </c>
@@ -14497,7 +14497,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A295" s="7" t="s">
         <v>727</v>
       </c>
@@ -14526,7 +14526,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A296" s="7" t="s">
         <v>728</v>
       </c>
@@ -14555,7 +14555,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A297" s="7" t="s">
         <v>730</v>
       </c>
@@ -14584,7 +14584,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A298" s="7" t="s">
         <v>773</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A299" s="7" t="s">
         <v>774</v>
       </c>
@@ -14642,7 +14642,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A300" s="7" t="s">
         <v>731</v>
       </c>
@@ -14671,7 +14671,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A301" s="7" t="s">
         <v>732</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A302" s="7" t="s">
         <v>733</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A303" s="7" t="s">
         <v>734</v>
       </c>
@@ -14758,7 +14758,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A304" s="7" t="s">
         <v>735</v>
       </c>
@@ -14781,7 +14781,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A305" s="7" t="s">
         <v>737</v>
       </c>
@@ -14804,7 +14804,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A306" s="7" t="s">
         <v>738</v>
       </c>
@@ -14827,7 +14827,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A307" s="7" t="s">
         <v>740</v>
       </c>
@@ -14850,7 +14850,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A308" s="7" t="s">
         <v>741</v>
       </c>
@@ -14873,7 +14873,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A309" s="7" t="s">
         <v>742</v>
       </c>
@@ -14896,7 +14896,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A310" s="7" t="s">
         <v>743</v>
       </c>
@@ -14919,7 +14919,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A311" s="7" t="s">
         <v>745</v>
       </c>
@@ -14942,7 +14942,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A312" s="7" t="s">
         <v>746</v>
       </c>
@@ -14973,7 +14973,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A313" s="7" t="s">
         <v>748</v>
       </c>
@@ -15008,7 +15008,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A314" s="7" t="s">
         <v>749</v>
       </c>
@@ -15039,7 +15039,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A315" s="7" t="s">
         <v>750</v>
       </c>
@@ -15070,7 +15070,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A316" s="7" t="s">
         <v>751</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A317" s="8" t="s">
         <v>752</v>
       </c>
@@ -15132,7 +15132,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A318" s="25" t="s">
         <v>1032</v>
       </c>
@@ -15158,7 +15158,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A319" s="25" t="s">
         <v>1037</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A320" s="25" t="s">
         <v>1041</v>
       </c>
@@ -15210,7 +15210,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A321" s="25" t="s">
         <v>1045</v>
       </c>
@@ -15236,7 +15236,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A322" s="25" t="s">
         <v>1049</v>
       </c>
@@ -15262,7 +15262,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A323" s="25" t="s">
         <v>1054</v>
       </c>
@@ -15288,7 +15288,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A324" s="25" t="s">
         <v>1058</v>
       </c>
@@ -15314,7 +15314,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A325" s="25" t="s">
         <v>1062</v>
       </c>
@@ -15340,7 +15340,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A326" s="25" t="s">
         <v>1067</v>
       </c>
@@ -15366,7 +15366,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A327" s="25" t="s">
         <v>1069</v>
       </c>
@@ -15392,7 +15392,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A328" s="25" t="s">
         <v>1073</v>
       </c>
@@ -15416,7 +15416,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A329" s="25" t="s">
         <v>1076</v>
       </c>
@@ -15442,7 +15442,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A330" s="25" t="s">
         <v>1081</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A331" s="25" t="s">
         <v>1085</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A332" s="25" t="s">
         <v>1089</v>
       </c>
@@ -15520,7 +15520,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A333" s="25" t="s">
         <v>1093</v>
       </c>
@@ -15546,7 +15546,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A334" s="25" t="s">
         <v>1096</v>
       </c>
@@ -15572,7 +15572,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A335" s="25" t="s">
         <v>1100</v>
       </c>
@@ -15598,7 +15598,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A336" s="25" t="s">
         <v>1103</v>
       </c>
@@ -15624,7 +15624,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A337" s="25" t="s">
         <v>1107</v>
       </c>
@@ -15650,7 +15650,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A338" s="25" t="s">
         <v>1111</v>
       </c>
@@ -15676,7 +15676,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A339" s="25" t="s">
         <v>1115</v>
       </c>
@@ -15702,7 +15702,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A340" s="25" t="s">
         <v>1118</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A341" s="25" t="s">
         <v>1121</v>
       </c>
@@ -15754,7 +15754,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A342" s="25" t="s">
         <v>1124</v>
       </c>
@@ -15780,7 +15780,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A343" s="25" t="s">
         <v>1128</v>
       </c>
@@ -15806,7 +15806,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A344" s="25" t="s">
         <v>1133</v>
       </c>
@@ -15832,7 +15832,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A345" s="25" t="s">
         <v>1137</v>
       </c>
@@ -15858,7 +15858,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A346" s="25" t="s">
         <v>1141</v>
       </c>
@@ -15884,7 +15884,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A347" s="25" t="s">
         <v>1146</v>
       </c>
@@ -15910,7 +15910,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A348" s="25" t="s">
         <v>1150</v>
       </c>
@@ -15936,7 +15936,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A349" s="25" t="s">
         <v>1154</v>
       </c>
@@ -15962,7 +15962,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A350" s="25" t="s">
         <v>1158</v>
       </c>
@@ -15988,7 +15988,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A351" s="25" t="s">
         <v>1161</v>
       </c>
@@ -16014,7 +16014,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A352" s="25" t="s">
         <v>1165</v>
       </c>
@@ -16040,7 +16040,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A353" s="25" t="s">
         <v>1169</v>
       </c>
@@ -16066,7 +16066,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A354" s="25" t="s">
         <v>1172</v>
       </c>
@@ -16092,7 +16092,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A355" s="25" t="s">
         <v>1176</v>
       </c>
@@ -16118,7 +16118,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A356" s="25" t="s">
         <v>1180</v>
       </c>
@@ -16138,7 +16138,7 @@
       <c r="J356" s="25"/>
       <c r="K356" s="25"/>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A357" s="25" t="s">
         <v>1181</v>
       </c>
@@ -16162,7 +16162,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A358" s="25" t="s">
         <v>1183</v>
       </c>
@@ -16188,7 +16188,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A359" s="25" t="s">
         <v>1187</v>
       </c>
@@ -16214,7 +16214,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A360" s="25" t="s">
         <v>1191</v>
       </c>
@@ -16240,7 +16240,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A361" s="25" t="s">
         <v>1194</v>
       </c>
@@ -16266,7 +16266,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A362" s="25" t="s">
         <v>1199</v>
       </c>
@@ -16292,7 +16292,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A363" s="25" t="s">
         <v>1203</v>
       </c>
@@ -16318,7 +16318,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A364" s="25" t="s">
         <v>1207</v>
       </c>
@@ -16344,7 +16344,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A365" s="25" t="s">
         <v>1210</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A366" s="25" t="s">
         <v>1213</v>
       </c>
@@ -16396,7 +16396,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A367" s="25" t="s">
         <v>1217</v>
       </c>
@@ -16422,7 +16422,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A368" s="25" t="s">
         <v>1221</v>
       </c>
@@ -16448,7 +16448,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A369" s="25" t="s">
         <v>1225</v>
       </c>
@@ -16474,7 +16474,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A370" s="25" t="s">
         <v>1229</v>
       </c>
@@ -16500,7 +16500,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A371" s="25" t="s">
         <v>1233</v>
       </c>
@@ -16526,7 +16526,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A372" s="25" t="s">
         <v>1237</v>
       </c>
@@ -16552,7 +16552,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A373" s="25" t="s">
         <v>1241</v>
       </c>
@@ -16578,7 +16578,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A374" s="25" t="s">
         <v>1244</v>
       </c>
@@ -16604,7 +16604,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A375" s="25" t="s">
         <v>1247</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A376" s="25" t="s">
         <v>1251</v>
       </c>
@@ -16656,7 +16656,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A377" s="25" t="s">
         <v>1255</v>
       </c>
@@ -16682,7 +16682,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A378" s="25" t="s">
         <v>1259</v>
       </c>
@@ -16708,7 +16708,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A379" s="25" t="s">
         <v>1263</v>
       </c>
@@ -16734,7 +16734,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A380" s="25" t="s">
         <v>1267</v>
       </c>
@@ -16760,7 +16760,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A381" s="25" t="s">
         <v>1271</v>
       </c>
@@ -16786,7 +16786,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A382" s="25" t="s">
         <v>1275</v>
       </c>
@@ -16812,7 +16812,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A383" s="25" t="s">
         <v>1279</v>
       </c>
@@ -16838,7 +16838,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A384" s="25" t="s">
         <v>1283</v>
       </c>
@@ -16864,7 +16864,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A385" s="25" t="s">
         <v>1287</v>
       </c>
@@ -16884,7 +16884,7 @@
       <c r="J385" s="25"/>
       <c r="K385" s="25"/>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A386" s="25" t="s">
         <v>1289</v>
       </c>
@@ -16910,7 +16910,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A387" s="25" t="s">
         <v>1293</v>
       </c>
@@ -16936,7 +16936,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A388" s="25" t="s">
         <v>1297</v>
       </c>
@@ -16962,7 +16962,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A389" s="25" t="s">
         <v>1300</v>
       </c>
@@ -16988,7 +16988,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A390" s="25" t="s">
         <v>1303</v>
       </c>
@@ -17014,7 +17014,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A391" s="25" t="s">
         <v>1307</v>
       </c>
@@ -17040,7 +17040,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A392" s="25" t="s">
         <v>1311</v>
       </c>
@@ -17066,7 +17066,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A393" s="25" t="s">
         <v>1314</v>
       </c>
@@ -17092,7 +17092,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A394" s="25" t="s">
         <v>1318</v>
       </c>
@@ -17118,7 +17118,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A395" s="25" t="s">
         <v>1322</v>
       </c>
@@ -17144,7 +17144,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A396" s="25" t="s">
         <v>1326</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A397" s="25" t="s">
         <v>1330</v>
       </c>
@@ -17196,7 +17196,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A398" s="25" t="s">
         <v>1334</v>
       </c>
@@ -17222,7 +17222,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A399" s="25" t="s">
         <v>1338</v>
       </c>
@@ -17248,7 +17248,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A400" s="25" t="s">
         <v>1343</v>
       </c>
@@ -17274,7 +17274,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A401" s="25" t="s">
         <v>1347</v>
       </c>
@@ -17300,7 +17300,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A402" s="25" t="s">
         <v>1350</v>
       </c>
@@ -17326,7 +17326,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A403" s="25" t="s">
         <v>1354</v>
       </c>
@@ -17350,7 +17350,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A404" s="25" t="s">
         <v>1357</v>
       </c>
@@ -17376,7 +17376,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A405" s="25" t="s">
         <v>1361</v>
       </c>
@@ -17402,7 +17402,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A406" s="25" t="s">
         <v>1365</v>
       </c>
@@ -17428,7 +17428,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A407" s="25" t="s">
         <v>1368</v>
       </c>
@@ -17454,7 +17454,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A408" s="25" t="s">
         <v>1373</v>
       </c>
@@ -17478,7 +17478,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A409" s="25" t="s">
         <v>1376</v>
       </c>
@@ -17504,7 +17504,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A410" s="25" t="s">
         <v>1379</v>
       </c>
@@ -17530,7 +17530,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A411" s="25" t="s">
         <v>1382</v>
       </c>
@@ -17556,7 +17556,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A412" s="25" t="s">
         <v>1385</v>
       </c>
@@ -17582,7 +17582,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A413" s="25" t="s">
         <v>1389</v>
       </c>
@@ -17608,7 +17608,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A414" s="25" t="s">
         <v>1392</v>
       </c>
@@ -17634,7 +17634,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A415" s="25" t="s">
         <v>1396</v>
       </c>
@@ -17660,7 +17660,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A416" s="25" t="s">
         <v>1400</v>
       </c>
@@ -17686,7 +17686,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A417" s="25" t="s">
         <v>1404</v>
       </c>
@@ -17712,7 +17712,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A418" s="25" t="s">
         <v>1408</v>
       </c>
@@ -17738,7 +17738,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A419" s="25" t="s">
         <v>1412</v>
       </c>
@@ -17764,7 +17764,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A420" s="25" t="s">
         <v>1416</v>
       </c>
@@ -17790,7 +17790,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A421" s="25" t="s">
         <v>1420</v>
       </c>
@@ -17816,7 +17816,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A422" s="25" t="s">
         <v>1424</v>
       </c>
@@ -17842,7 +17842,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A423" s="25" t="s">
         <v>1428</v>
       </c>
@@ -17868,7 +17868,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A424" s="25" t="s">
         <v>1433</v>
       </c>
@@ -17894,7 +17894,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A425" s="25" t="s">
         <v>1437</v>
       </c>
@@ -17920,7 +17920,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A426" s="25" t="s">
         <v>1441</v>
       </c>
@@ -17946,7 +17946,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A427" s="25" t="s">
         <v>1445</v>
       </c>
@@ -17972,7 +17972,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A428" s="25" t="s">
         <v>1449</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A429" s="25" t="s">
         <v>1453</v>
       </c>
@@ -18024,7 +18024,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A430" s="25" t="s">
         <v>1455</v>
       </c>
@@ -18050,7 +18050,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A431" s="25" t="s">
         <v>1460</v>
       </c>
@@ -18076,7 +18076,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A432" s="25" t="s">
         <v>1464</v>
       </c>
@@ -18102,7 +18102,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A433" s="25" t="s">
         <v>1467</v>
       </c>
@@ -18128,7 +18128,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A434" s="25" t="s">
         <v>1470</v>
       </c>
@@ -18154,7 +18154,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A435" s="25" t="s">
         <v>1474</v>
       </c>
@@ -18180,7 +18180,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A436" s="25" t="s">
         <v>1478</v>
       </c>
@@ -18206,7 +18206,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A437" s="25" t="s">
         <v>1482</v>
       </c>
@@ -18232,7 +18232,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A438" s="25" t="s">
         <v>1486</v>
       </c>
@@ -18258,7 +18258,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A439" s="25" t="s">
         <v>1490</v>
       </c>

</xml_diff>